<commit_message>
inicio SOR, separación html en secciones
</commit_message>
<xml_diff>
--- a/app/tables/tabla_gaussSeidel.xlsx
+++ b/app/tables/tabla_gaussSeidel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,12 +458,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[1;3;6]</t>
+          <t>[2.5 0.25 1;1.66666666666667 3.16666666666667 2.16666666666667;1.77083333333333 2.80208333333333 2.58333333333333]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>13.2</t>
         </is>
       </c>
     </row>
@@ -475,12 +475,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[4.39;2.895;6.82125]</t>
+          <t>[0.364583333333333 -1.27604166666667 -0.416666666666667;2.79513888888889 3.71701388888889 3.18055555555556;2.82335069444444 3.61827256944444 3.21527777777778]</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.772209567198178</t>
+          <t>10.4530612244898</t>
         </is>
       </c>
     </row>
@@ -492,12 +492,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[4.8591625;2.88320625;6.9355921875]</t>
+          <t>[-1.00802951388889 -2.09689670138889 -1.49305555555556;3.53479456018518 4.12821903935185 3.79282407407407;3.49631980613426 4.02850567853009 3.7349537037037]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.0965521321832722</t>
+          <t>2.47407129452994</t>
         </is>
       </c>
     </row>
@@ -509,12 +509,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[4.924455484375;2.8815500859375;6.95150139257813]</t>
+          <t>[-1.89925582320602 -2.61041711877894 -2.21209490740741;4.0167839144483 4.40219379943094 4.18557098765432;3.93283891089169 4.2809622493791 4.08616657021605]</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.0132589246835861</t>
+          <t>0.991019001341996</t>
         </is>
       </c>
     </row>
@@ -526,12 +526,471 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[4.93354029291016;2.88131972868164;6.95371500539795]</t>
+          <t>[-2.47900739128207 -2.94212647426276 -2.68226152584877;4.3305317757061 4.58125727461199 4.4404799221965;4.21674667562477 4.44351472776123 4.31629347310635]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.0018414379929583</t>
+          <t>0.521896549517097</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>[-2.85627216959196 -3.1577003198396 -2.98850667820055;4.53472366712384 4.69788109193286 4.60628887328264;4.40148918921401 4.54909242691654 4.46624445555469]</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.302826485080389</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>[-3.10178734494989 -3.29795703240792 -3.18783888273933;4.66761003176426 4.77378928378585 4.71418517923377;4.52171458265262 4.61777582430848 4.56385300690364]</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.1842101154533</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>[-3.2615648151495 -3.38922987499363 -3.31756538787715;4.75409077965756 4.82319061261101 4.78440142410082;4.59995531455405 4.66247101871827 4.62737801139801]</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0.115021163090169</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>[-3.3655457420202 -3.44862846881739 -3.40199007377462;4.81037127558779 4.85534047609188 4.83009704728341;4.65087326986568 4.6915576739879 4.66871953428829]</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0.0729358060726012</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>[-3.43321509162368 -3.48728419406286 -3.4569325526067;4.84699784943817 4.87626318371059 4.85983511268975;4.68400996990526 4.71048682536164 4.69562406720675]</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0.0466883823364352</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>[-3.47725337203126 -3.51244080046376 -3.49268836812069;4.8708339197033 4.88987939608224 4.87918823421267;4.70557487759371 4.72280565126929 4.71313317152226]</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0.0300641513603654</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>[-3.50591287857433 -3.52881237269632 -3.51595776142063;4.88634610611727 4.89874063991933 4.89178297902671;4.71960902257964 4.73082257295537 4.72452785613122]</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0.0194322435395551</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>[-3.52456409087777 -3.53946676641718 -3.53110116233564;4.89644122348857 4.90450741545223 4.89997946553522;4.72874225092646 4.73603987514768 4.73194336007597]</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>0.0125905250928361</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>[-3.53670204307966 -3.54640049916301 -3.5409562791894;4.9030109868987 4.90826035358406 4.90531362611361;4.73468603020011 4.73943522358087 4.73676926796498]</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>0.008170323437991</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>[-3.54460125527408 -3.55091287697848 -3.54736985356769;4.9072864984827 4.91070271405551 4.9087850243843;4.73855415992562 4.74164486959767 4.73990990238373]</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>0.0053072650126202</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>[-3.54974195382484 -3.55384947034047 -3.55154371948009;4.91006894256229 4.91229216862737 4.91104416258944;4.74107148549995 4.74308287680595 4.7419537840277]</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0.0034497285738093</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>[-3.55308744967169 -3.5557605648735 -3.55426001395593;4.91187971886447 4.91332656378134 4.91251437863267;4.74270972632869 4.7440187121006 4.74328391406429]</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>0.0022432749399862</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>[-3.5552646523127 -3.55700427888631 -3.55602774100664;4.91305814715368 4.91399973390744 4.91347117499371;4.74377587090701 4.74462774082708 4.74414954438072]</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>0.0014591476615323</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>[-3.55668154581877 -3.55781367084412 -3.55717815343565;4.91382505206134 4.91443782375823 4.91409384489364;4.74446970312139 4.74502408833802 4.74471288467387]</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>0.0009492780527309</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>[-3.5576036406067 -3.55834041198768 -3.55792682600717;4.91432414321757 4.91472292660212 4.91449906989247;4.7449212395748 4.74528202584177 4.74507949878136]</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>0.0006176436879472</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>[-3.55820372720058 -3.55868320787248 -3.55841405181003;4.91464894487125 4.91490846760802 4.91476278474313;4.74521509328255 4.74544988801829 4.74531808619549]</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0.0004018975321017</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>[-3.55859425529471 -3.55890629471516 -3.55873113165509;4.91486032131605 4.91502921514039 4.91493440673748;4.74540632923018 4.74555913041188 4.74547335560006]</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>0.0002615254675413</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>[-3.55884840560213 -3.55905147656123 -3.55893748285314;4.91499788219639 4.91510779597218 4.91504609596875;4.74553078295223 4.74563022385773 4.74557440279102]</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>0.0001701870476013</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>[-3.55901380312341 -3.559145958908 -3.55907177337208;4.91508740492357 4.91515893529571 4.91511878178288;4.74561177572124 4.74567649049357 4.74564016291183]</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>0.0001107510993776</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>[-3.55912144155329 -3.55920744671857 -3.55915916779307;4.91514566508199 4.91519221606345 4.91516608471008;4.74566448470031 4.74570660018324 4.74568295869315]</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>7.20734747345283e-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>[-3.55919149116165 -3.55924746213921 -3.55921604287913;4.91518357999105 4.91521387472893 4.9151968688039;4.74569878697827 4.74572619515477 4.74571080959848]</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>4.69036560347471e-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>[-3.55923707848242 -3.55927350362408 -3.55925305640216;4.9152082544919 4.91522796989026 4.91521690266836;4.74572111042854 4.74573894729249 4.74572893458426]</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>3.05239279149347e-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>[-3.55926674608319 -3.55929045106394 -3.5592771442934;4.91522431231737 4.91523714282721 4.91522994043156;4.74573563822265 4.74574724620816 4.74574073007549]</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>1.98644141255277e-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>[-3.55928605334936 -3.55930148022449 -3.55929282036141;4.91523476252913 4.9152431124483 4.91523842522836;4.74574509271107 4.74575264702823 4.74574840641879]</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>1.29274288221886e-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>[-3.55929861825238 -3.55930865785034 -3.55930302213067;4.91524156338308 4.91524699739552 4.91524394701731;4.74575124556197 4.74575616180758 4.74575340207734]</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>8.41296796716408e-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>[-3.55930679531829 -3.55931332895043 -3.55930966130165;4.9152459892852 4.91524952566569 4.91524754052154;4.74575524975263 4.7457584491776 4.74575665318315]</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>5.47503325497692e-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>[-3.55931211684021 -3.55931636883807 -3.55931398198273;4.91524886960137 4.91525117102911 4.91524987912463;4.74575785562479 4.74575993776651 4.74575876895805]</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>3.56307183135093e-06</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
separación de las rutas en secciones
</commit_message>
<xml_diff>
--- a/app/tables/tabla_gaussSeidel.xlsx
+++ b/app/tables/tabla_gaussSeidel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[1;3;6]</t>
+          <t>[0.75;0.03125]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -475,12 +475,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[4.39;2.895;6.82125]</t>
+          <t>[0.7109375;0.0556640625]</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.772209567198178</t>
+          <t>0.43859649122807</t>
         </is>
       </c>
     </row>
@@ -492,12 +492,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[4.8591625;2.88320625;6.9355921875]</t>
+          <t>[0.680419921875;0.074737548828125]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.0965521321832722</t>
+          <t>0.255206206614945</t>
         </is>
       </c>
     </row>
@@ -509,12 +509,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[4.924455484375;2.8815500859375;6.95150139257813]</t>
+          <t>[0.656578063964844;0.0896387100219727]</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.0132589246835861</t>
+          <t>0.166235783515794</t>
         </is>
       </c>
     </row>
@@ -526,12 +526,692 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[4.93354029291016;2.88131972868164;6.95371500539795]</t>
+          <t>[0.637951612472534;0.101280242204666]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.0018414379929583</t>
+          <t>0.114943763258073</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>[0.623399697244167;0.110375189222395]</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.082400284718007</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>[0.612031013472006;0.117480616579996]</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.0604816995726498</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>[0.603149229275004;0.123031731703122]</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0.0451193773043911</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>[0.596210335371097;0.127368540393064]</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0.0340492925219874</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>[0.59078932450867;0.130756672182081]</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0.0259117315581354</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>[0.586554159772398;0.133403650142251]</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0.0198418705736099</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>[0.583245437322186;0.135471601673634]</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0.0152648341485215</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>[0.580660497907958;0.137087188807526]</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>0.0117851066022</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>[0.578641013990592;0.13834936625588]</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>0.0091231169503097</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>[0.57706329218015;0.139335442387406]</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>0.0070769942997316</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>[0.575830697015742;0.140105814365161]</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0.0054985011239223</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>[0.574867732043549;0.140707667472782]</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>0.004277329860062</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>[0.574115415659022;0.141177865213111]</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>0.0033305344263361</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>[0.573527668483611;0.141545207197743]</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>0.0025952272910149</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>[0.573068491002821;0.141832193123237]</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>0.0020234187963544</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>[0.572709758595954;0.142056400877529]</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0.001578300962906</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>[0.572429498903089;0.142231563185569]</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>0.0012315290932439</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>[0.572210546018038;0.142368408738726]</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>0.0009612072956989</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>[0.572039489076593;0.14247531932713]</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>0.0007503797072265</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>[0.571905850841088;0.14255884322432]</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0.0005858906771497</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>[0.5718014459696;0.142624096269]</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>0.0004575176732894</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>[0.57171987966375;0.142675075210156]</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>0.0003573079676401</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>[0.571656155987305;0.142714902507935]</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>0.0002790689485008</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>[0.571606371865082;0.142746017584324]</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>0.0002179750925165</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>[0.571567478019595;0.142770326237753]</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>0.0001702640462463</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>[0.571537092202809;0.142789317373245]</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>0.0001330010944856</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>[0.571513353283444;0.142804154197847]</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>0.0001038963095021</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>[0.571494807252691;0.142815745467068]</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>8.11624039281694e-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>[0.571480318166165;0.142824801146147]</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>6.34041077330991e-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>[0.571468998567316;0.142831875895427]</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>4.9532005625325e-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>[0.571460155130716;0.142837403043303]</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>3.86953820041757e-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>[0.571453246195872;0.14284172112758]</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>3.02298533192804e-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>[0.571447848590525;0.142845094630922]</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2.36165151527095e-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>[0.571443631711347;0.142847730180408]</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>1.84500620518261e-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>[0.57144033727449;0.142849789203444]</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>1.44139032145282e-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>[0.571437763495696;0.14285139781519]</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>1.12607350806341e-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>[0.571435752731012;0.142852654543117]</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>8.79737188736098e-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>[0.571434181821103;0.14285363636181]</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>6.87289955001289e-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>[0.571432954547737;0.142854403407664]</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>5.36942394247e-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>[0.571431995740419;0.142855002662238]</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>4.19484485835463e-06</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
control de coma por punto decimal
</commit_message>
<xml_diff>
--- a/app/tables/tabla_gaussSeidel.xlsx
+++ b/app/tables/tabla_gaussSeidel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[2.5;0.666666666666667]</t>
+          <t>[1.6;1.75;1]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -475,27 +475,10 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[-0.166666666666667;0.666666666666667]</t>
+          <t>[1.6;1.75;1]</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>[-0.166666666666667;0.666666666666667]</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>

<commit_message>
Centro de Ayudas y corrección métodos Newton y Gauss-Seidel
</commit_message>
<xml_diff>
--- a/app/tables/tabla_gaussSeidel.xlsx
+++ b/app/tables/tabla_gaussSeidel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,12 +458,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[0;0.5]</t>
+          <t>[1;3;6]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>inf</t>
+          <t>1.0</t>
         </is>
       </c>
     </row>
@@ -475,12 +475,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[0.333333333333333;0.333333333333333]</t>
+          <t>[4.39;2.895;6.82125]</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.772209567198178</t>
         </is>
       </c>
     </row>
@@ -492,216 +492,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[0.444444444444444;0.277777777777778]</t>
+          <t>[4.8591625;2.88320625;6.9355921875]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.25</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>[0.481481481481481;0.259259259259259]</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0.0769230769230769</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>[0.493827160493827;0.253086419753086]</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>0.025</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>[0.497942386831276;0.251028806584362]</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>0.0082644628099173</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>[0.499314128943759;0.250342935528121]</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>0.0027472527472527</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>[0.499771376314586;0.250114311842707]</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>0.0009149130832571</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>[0.499923792104862;0.250038103947569]</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>0.0003048780487804</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>[0.499974597368287;0.250012701315856]</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>0.0001016156894624</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>[0.499991532456096;0.250004233771952]</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>3.3870749220958e-05</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>[0.499997177485365;0.250001411257317]</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>1.12901222720193e-05</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>[0.499999059161788;0.250000470419106]</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>3.76335992777886e-06</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>[0.499999686387263;0.250000156806369]</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>1.25445173560849e-06</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>[0.499999895462421;0.25000005226879]</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>4.18150403686329e-07</t>
+          <t>0.0965521321832722</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
se corrige SOR y Jacobi cuando la diagonal de A es cero
</commit_message>
<xml_diff>
--- a/app/tables/tabla_gaussSeidel.xlsx
+++ b/app/tables/tabla_gaussSeidel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,12 +458,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[1;3;6]</t>
+          <t>[1;0.75]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>10.0</t>
         </is>
       </c>
     </row>
@@ -475,12 +475,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[4.39;2.895;6.82125]</t>
+          <t>[1.375;0.5625]</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.772209567198178</t>
+          <t>0.333333333333333</t>
         </is>
       </c>
     </row>
@@ -492,12 +492,1661 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[4.8591625;2.88320625;6.9355921875]</t>
+          <t>[1.65625;0.421875]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.0965521321832722</t>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>[1.8671875;0.31640625]</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>[2.025390625;0.2373046875]</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>[2.14404296875;0.177978515625]</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>[2.2330322265625;0.13348388671875]</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>[2.29977416992188;0.100112915039062]</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>[2.34983062744141;0.0750846862792969]</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>[2.38737297058105;0.0563135147094727]</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>[2.41552972793579;0.0422351360321045]</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>[2.43664729595184;0.0316763520240784]</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>[2.45248547196388;0.0237572640180588]</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>[2.46436410397291;0.0178179480135441]</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>[2.47327307797968;0.0133634610101581]</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>[2.47995480848476;0.0100225957576185]</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>[2.48496610636357;0.00751694681821391]</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>[2.48872457977268;0.00563771011366043]</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>[2.49154343482951;0.00422828258524532]</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>[2.49365757612213;0.00317121193893399]</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>[2.4952431820916;0.00237840895420049]</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>[2.4964323865687;0.00178380671565037]</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>[2.49732428992652;0.00133785503673778]</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>[2.49799321744489;0.00100339127755333]</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>[2.49849491308367;0.000752543458165]</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>[2.49887118481275;0.00056440759362375]</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>[2.49915338860956;0.000423305695217813]</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>[2.49936504145717;0.00031747927141336]</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>[2.49952378109288;0.00023810945356002]</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>[2.49964283581966;0.000178582090170015]</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>[2.49973212686474;0.000133936567627511]</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>[2.49979909514856;0.000100452425720633]</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>[2.49984932136142;7.5339319290475e-05]</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>[2.49988699102106;5.65044894678562e-05]</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>[2.4999152432658;4.23783671008922e-05]</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>[2.49993643244935;3.17837753256691e-05]</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>[2.49995232433701;2.38378314942518e-05]</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>[2.49996424325276;1.78783736206889e-05]</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>[2.49997318243957;1.34087802155167e-05]</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>[2.49997988682968;1.00565851616375e-05]</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>[2.49998491512226;7.54243887122812e-06]</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>[2.49998868634169;5.65682915342109e-06]</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>[2.49999151475627;4.24262186506582e-06]</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>[2.4999936360672;3.18196639879936e-06]</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>[2.4999952270504;2.38647479909952e-06]</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>[2.4999964202878;1.78985609932464e-06]</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>[2.49999731521585;1.34239207449348e-06]</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>[2.49999798641189;1.00679405587011e-06]</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>[2.49999848980892;7.55095541902583e-07]</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>[2.49999886735669;5.66321656426938e-07]</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>[2.49999915051752;4.24741242320203e-07]</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>[2.49999936288814;3.18555931740152e-07]</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>[2.4999995221661;2.38916948805114e-07]</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>[2.49999964162458;1.79187711603836e-07]</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>[2.49999973121843;1.34390783702877e-07]</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>[2.49999979841382;1.00793087777158e-07]</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>[2.49999984881037;7.55948158328682e-08]</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>[2.49999988660778;5.66961118746512e-08]</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>[2.49999991495583;4.25220839059884e-08]</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>[2.49999993621687;3.18915629294913e-08]</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>[2.49999995216266;2.39186721971185e-08]</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>[2.49999996412199;1.79390041478388e-08]</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>[2.49999997309149;1.34542531108791e-08]</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>[2.49999997981862;1.00906898331593e-08]</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>[2.49999998486397;7.56801737486951e-09]</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>[2.49999998864797;5.67601303115213e-09]</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>[2.49999999148598;4.2570097733641e-09]</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>[2.49999999361449;3.19275733002308e-09]</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>[2.49999999521086;2.39456799751731e-09]</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>[2.49999999640815;1.79592599813798e-09]</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>[2.49999999730611;1.34694449860348e-09]</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>[2.49999999797958;1.01020837395261e-09]</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>[2.49999999848469;7.5765628046446e-10]</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>[2.49999999886352;5.68242210348345e-10]</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>[2.49999999914764;4.26181657761259e-10]</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>[2.49999999936073;3.19636243320944e-10]</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>[2.49999999952055;2.39727182490708e-10]</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>[2.49999999964041;1.79795386868031e-10]</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>[2.49999999973031;1.34846540151023e-10]</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>[2.49999999979773;1.01134905113267e-10]</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>[2.4999999998483;7.58511788349506e-11]</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>[2.49999999988622;5.6888384126213e-11]</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>[2.49999999991467;4.26662880946597e-11]</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>[2.499999999936;3.19997160709948e-11]</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>[2.499999999952;2.39997870532461e-11]</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>86</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>[2.499999999964;1.79998402899346e-11]</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>[2.499999999973;1.34998802174509e-11]</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>[2.49999999997975;1.01249101630882e-11]</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>[2.49999999998481;7.59368262231615e-12]</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>[2.49999999998861;5.69526196673711e-12]</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>[2.49999999999146;4.27144647505283e-12]</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>[2.49999999999359;3.20358485628962e-12]</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>[2.49999999999519;2.40268864221722e-12]</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>[2.4999999999964;1.80201648166291e-12]</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>95</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>[2.4999999999973;1.35151236124719e-12]</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>[2.49999999999797;1.01363427093539e-12]</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>[2.49999999999848;7.60225703201542e-13]</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>[2.49999999999886;5.70169277401156e-13]</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>[2.49999999999914;4.27626958050867e-13]</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>[2.49999999999936;3.2072021853815e-13]</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>0.333333333333333</t>
         </is>
       </c>
     </row>

</xml_diff>